<commit_message>
Se agrega el campo para EGMA
</commit_message>
<xml_diff>
--- a/Base_organizada/BBDD_AG_JARPMJ_2022/Estructura.xlsx
+++ b/Base_organizada/BBDD_AG_JARPMJ_2022/Estructura.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bambooanalytics-my.sharepoint.com/personal/francisco_echeverri_wadua_com_co/Documents/Documentos/Prueba_GIT_AG/Proyecto_AulaGlobal/Base_organizada/BBDD_AG_JARPMJ_2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="920" documentId="11_AD4D2F04E46CFB4ACB3E209E1552FDD2693EDF25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BF2EA49-CE24-487E-AB46-DE8FDB2A16E2}"/>
+  <xr:revisionPtr revIDLastSave="924" documentId="11_AD4D2F04E46CFB4ACB3E209E1552FDD2693EDF25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45CD8192-8493-45EB-B808-B1AB75B01DA3}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-2085" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2°" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="399">
   <si>
     <t>ID</t>
   </si>
@@ -1318,6 +1318,9 @@
   </si>
   <si>
     <t>id_global</t>
+  </si>
+  <si>
+    <t>egma_items</t>
   </si>
 </sst>
 </file>
@@ -1733,16 +1736,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="24" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>397</v>
       </c>
@@ -1814,6 +1819,9 @@
       </c>
       <c r="X1" s="3" t="s">
         <v>221</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -1828,9 +1836,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B85E7FBF-3E4B-42ED-8B6D-E36417E6C3AA}">
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Z1" sqref="Z1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1841,7 +1851,7 @@
     <col min="18" max="25" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>397</v>
       </c>
@@ -1916,6 +1926,9 @@
       </c>
       <c r="Y1" s="3" t="s">
         <v>323</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -1930,9 +1943,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{278AF3AC-D490-4241-AABC-78DACEC6BFDF}">
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1943,7 +1958,7 @@
     <col min="18" max="24" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>397</v>
       </c>
@@ -2015,6 +2030,9 @@
       </c>
       <c r="X1" s="3" t="s">
         <v>323</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -2028,10 +2046,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE46E8E4-5592-4676-8D4A-F249FD9FEFD4}">
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2043,7 +2061,7 @@
     <col min="18" max="24" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>397</v>
       </c>
@@ -2115,6 +2133,9 @@
       </c>
       <c r="X1" s="3" t="s">
         <v>323</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -5596,6 +5617,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101007E6519502A214D43B3DDFCF5E94F901E" ma:contentTypeVersion="6" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="90f6c4560d8bc755c62d8c2203e7a644">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3eff0a0a-75ec-4759-8be4-4c323b0f0df5" xmlns:ns3="cd170719-9bd0-436b-b4b8-eee07325531c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64ddfcc38bb4a68bf603592444bf132" ns2:_="" ns3:_="">
     <xsd:import namespace="3eff0a0a-75ec-4759-8be4-4c323b0f0df5"/>
@@ -5772,22 +5808,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C74A6BC-21F1-4719-A2D5-65CA0F8C2D1D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68DE72E2-C7DF-4BFF-AC6A-0054F74EB776}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{454A1F66-50AE-4DD6-85A3-C6084E539166}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5804,21 +5842,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68DE72E2-C7DF-4BFF-AC6A-0054F74EB776}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C74A6BC-21F1-4719-A2D5-65CA0F8C2D1D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>